<commit_message>
Corrected ingest and Cal sheets
Corrected FLORT resolution and scattering angle Cal values to 1.076, 124
corrected recovered data sources
Changed WFP eng data reference designator from STC to WFP
</commit_message>
<xml_diff>
--- a/CE09OSPM/Omaha_Cal_Info_CE09OSPM_00001.xlsx
+++ b/CE09OSPM/Omaha_Cal_Info_CE09OSPM_00001.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gauls\Documents\Project Info\WHOI\Marine Integration - OOI\OOInet Migration\Integration\Cal and Ingest Sheets\Sheets from -test 2015-08-19\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-12" yWindow="-12" windowWidth="12720" windowHeight="12408" tabRatio="377" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405" tabRatio="377"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -35,7 +30,7 @@
     <definedName name="_FilterDatabase_1_1_1">Moorings!$A$1:$J$84</definedName>
     <definedName name="_FilterDatabase_2">Asset_Cal_Info!$A$1:$F$399</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -729,7 +724,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -764,7 +759,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -975,28 +970,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.88671875"/>
-    <col min="2" max="2" width="39.44140625"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="17.44140625"/>
-    <col min="7" max="7" width="18.6640625"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875"/>
-    <col min="10" max="10" width="12.6640625"/>
-    <col min="11" max="11" width="51.6640625"/>
+    <col min="1" max="1" width="37.85546875"/>
+    <col min="2" max="2" width="39.42578125"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="17.42578125"/>
+    <col min="7" max="7" width="18.7109375"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875"/>
+    <col min="10" max="10" width="12.7109375"/>
+    <col min="11" max="11" width="51.7109375"/>
     <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="1026" width="8.6640625"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="1026" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="31.2">
+    <row r="1" spans="1:13" ht="31.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1026,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.6">
+    <row r="2" spans="1:13" ht="15.75">
       <c r="A2" s="12" t="s">
         <v>34</v>
       </c>
@@ -1090,27 +1085,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625"/>
-    <col min="9" max="9" width="11.88671875"/>
-    <col min="10" max="10" width="14.44140625"/>
-    <col min="11" max="11" width="13.44140625"/>
-    <col min="12" max="1026" width="8.6640625"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125"/>
+    <col min="9" max="9" width="11.85546875"/>
+    <col min="10" max="10" width="14.42578125"/>
+    <col min="11" max="11" width="13.42578125"/>
+    <col min="12" max="1026" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6">
+    <row r="1" spans="1:7" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1431,7 +1426,7 @@
         <v>61</v>
       </c>
       <c r="F17" s="24">
-        <v>1.08</v>
+        <v>1.0760000000000001</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>33</v>
@@ -1638,7 +1633,7 @@
         <v>64</v>
       </c>
       <c r="F26" s="24">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="G26" s="9" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
redmine #9273 cal sheets for CE09OSPM multiple deployments changed/added to repo.
</commit_message>
<xml_diff>
--- a/CE09OSPM/Omaha_Cal_Info_CE09OSPM_00001.xlsx
+++ b/CE09OSPM/Omaha_Cal_Info_CE09OSPM_00001.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405" tabRatio="377"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12720" windowHeight="12405" tabRatio="377" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="68">
   <si>
     <t>Ref Des</t>
   </si>
@@ -321,6 +321,9 @@
       </rPr>
       <t xml:space="preserve"> Sheet  or QCT capture file as M2d</t>
     </r>
+  </si>
+  <si>
+    <t>Constant; chi factor</t>
   </si>
 </sst>
 </file>
@@ -970,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1043,7 +1046,7 @@
         <v>4.027777777777778E-2</v>
       </c>
       <c r="F2" s="4">
-        <v>41920</v>
+        <v>41866</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>55</v>
@@ -1085,8 +1088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1097,7 +1100,7 @@
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="58.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.42578125"/>
     <col min="9" max="9" width="11.85546875"/>
     <col min="10" max="10" width="14.42578125"/>
@@ -1429,7 +1432,7 @@
         <v>1.0760000000000001</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7">

</xml_diff>